<commit_message>
Added button to unallocate a student from a project
</commit_message>
<xml_diff>
--- a/storage/exports/ProjectAllocations.xlsx
+++ b/storage/exports/ProjectAllocations.xlsx
@@ -32,19 +32,19 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>Amina Durgan</t>
+    <t>Aimee Collins</t>
   </si>
   <si>
     <t>UoG</t>
   </si>
   <si>
-    <t>Deanna Hills</t>
-  </si>
-  <si>
-    <t>Roberta Lehner</t>
-  </si>
-  <si>
-    <t>Immanuel Wuckert</t>
+    <t>Ronny Dickinson</t>
+  </si>
+  <si>
+    <t>Al Herzog</t>
+  </si>
+  <si>
+    <t>Loyal Steuber</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.85376" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11.425781" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>
@@ -453,13 +453,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -487,13 +487,13 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hiding button to submit if javascript is not enabled
</commit_message>
<xml_diff>
--- a/storage/exports/ProjectAllocations.xlsx
+++ b/storage/exports/ProjectAllocations.xlsx
@@ -32,19 +32,19 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>Aimee Collins</t>
+    <t>Nikki Klocko</t>
   </si>
   <si>
     <t>UoG</t>
   </si>
   <si>
-    <t>Ronny Dickinson</t>
-  </si>
-  <si>
-    <t>Al Herzog</t>
-  </si>
-  <si>
-    <t>Loyal Steuber</t>
+    <t>Sheldon McGlynn</t>
+  </si>
+  <si>
+    <t>Yvette Mohr</t>
+  </si>
+  <si>
+    <t>Candace Renner</t>
   </si>
 </sst>
 </file>
@@ -436,13 +436,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -470,13 +470,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>

<commit_message>
Students can now select their degree type. Will ask them when they log in if it isn't set.
</commit_message>
<xml_diff>
--- a/storage/exports/ProjectAllocations.xlsx
+++ b/storage/exports/ProjectAllocations.xlsx
@@ -32,19 +32,19 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>Nikki Klocko</t>
+    <t>Concepcion Hammes</t>
   </si>
   <si>
     <t>UoG</t>
   </si>
   <si>
-    <t>Sheldon McGlynn</t>
-  </si>
-  <si>
-    <t>Yvette Mohr</t>
-  </si>
-  <si>
-    <t>Candace Renner</t>
+    <t>Pierce Rempel</t>
+  </si>
+  <si>
+    <t>Estella Rogahn</t>
+  </si>
+  <si>
+    <t>Jamil Thompson</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.85376" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11.425781" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>
@@ -453,13 +453,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -470,13 +470,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>